<commit_message>
Cambio y correcion en numero de cuentas por cobrar cliente
</commit_message>
<xml_diff>
--- a/Cuentas Contables-Condominios.xlsx
+++ b/Cuentas Contables-Condominios.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PATRICIO.CORDOVA\Downloads\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VisualStudio\ProyectoConjuntos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C07EBEE-1D37-483A-88FE-596C32E70CB7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D969A74-7891-40C7-A518-D72555A75544}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8484" xr2:uid="{361379C8-8CC7-4C27-ABB9-CEE8DCC6075B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8490" xr2:uid="{361379C8-8CC7-4C27-ABB9-CEE8DCC6075B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
   <si>
     <t>Nombre</t>
   </si>
@@ -138,9 +138,6 @@
     <t>Selección deuda mes (enero, febrero)</t>
   </si>
   <si>
-    <t>Generar Adeudo</t>
-  </si>
-  <si>
     <t>Generar de forma general de todo el edificio</t>
   </si>
   <si>
@@ -160,6 +157,18 @@
   </si>
   <si>
     <t>Plan de Cuentas Contables</t>
+  </si>
+  <si>
+    <t>Generar Adeudo / Ctas.por Cobrar Clientes</t>
+  </si>
+  <si>
+    <t>Departamento 101</t>
+  </si>
+  <si>
+    <t>1.1.3.02</t>
+  </si>
+  <si>
+    <t>Departamento 102</t>
   </si>
 </sst>
 </file>
@@ -203,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -213,11 +222,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -237,7 +249,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -536,27 +548,27 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.21875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="3"/>
-    <col min="9" max="9" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="3"/>
+    <col min="9" max="9" width="39.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -570,10 +582,10 @@
         <v>16</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -585,10 +597,10 @@
       </c>
       <c r="D3" s="3"/>
       <c r="I3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -600,10 +612,10 @@
       </c>
       <c r="D4" s="3"/>
       <c r="I4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -614,17 +626,17 @@
         <v>3</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" t="s">
         <v>40</v>
-      </c>
-      <c r="J5" t="s">
-        <v>41</v>
       </c>
       <c r="K5">
         <v>8000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -637,17 +649,17 @@
       <c r="D6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="5" t="s">
         <v>20</v>
       </c>
       <c r="J6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K6">
         <v>8000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -659,7 +671,7 @@
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -673,7 +685,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -690,7 +702,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
@@ -704,7 +716,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>27</v>
       </c>
@@ -718,7 +730,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>28</v>
       </c>
@@ -729,17 +741,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I14" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
@@ -749,25 +761,36 @@
       <c r="C15" s="3">
         <v>3</v>
       </c>
+      <c r="D15" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="I15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>40</v>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="C17" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>13</v>
       </c>
@@ -777,13 +800,13 @@
       <c r="C19" s="3">
         <v>1</v>
       </c>
-      <c r="I19" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="J19" s="5"/>
+      <c r="I19" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J19" s="6"/>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
@@ -794,13 +817,13 @@
         <v>1</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>23</v>
       </c>
@@ -817,7 +840,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
@@ -828,7 +851,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>

</xml_diff>